<commit_message>
fixed issues in downloadable files
</commit_message>
<xml_diff>
--- a/storage/app/public/downloads/sample-files/bulkdownloadableproductupload.xlsx
+++ b/storage/app/public/downloads/sample-files/bulkdownloadableproductupload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t xml:space="preserve">categories_slug</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t xml:space="preserve">Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nike</t>
   </si>
   <si>
     <t xml:space="preserve">downloadable</t>
@@ -309,31 +306,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AT2" activeCellId="0" sqref="AT2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -551,11 +545,8 @@
       <c r="AD2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="AG2" s="0" t="n">
         <v>1</v>
@@ -576,19 +567,19 @@
         <v>32</v>
       </c>
       <c r="AM2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="AN2" s="0" t="s">
+      <c r="AO2" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>